<commit_message>
Add export import dosen, bulk insert pembelajaran and few fixes
</commit_message>
<xml_diff>
--- a/public/files/KRS.xlsx
+++ b/public/files/KRS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>nim</t>
   </si>
@@ -40,14 +40,131 @@
   </si>
   <si>
     <t>tahun_ajaran</t>
+  </si>
+  <si>
+    <t>kd_dosen</t>
+  </si>
+  <si>
+    <t>AKHMAD YAZID ARIFIN</t>
+  </si>
+  <si>
+    <t>REGULER</t>
+  </si>
+  <si>
+    <t>IF1007</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>Mina Ismu Rahayu, M.T.</t>
+  </si>
+  <si>
+    <t>Grafika Komputer</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Catatan: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Masukkan </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">BL </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">pada kolom </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kd_dosen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jika nama dosen </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Belum Ditentukan -</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -92,10 +209,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,58 +514,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="11" max="11" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>20192</v>
+      </c>
+      <c r="B2">
+        <v>1213045</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changes made after sidang
</commit_message>
<xml_diff>
--- a/public/files/KRS.xlsx
+++ b/public/files/KRS.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -600,28 +598,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>